<commit_message>
Chiarimenti per casi ID [29, 37, 63, 65]
Aggiunti chiarimenti per i casi con  ID [29, 37, 63, 65]
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111NOLEXXXXXXX/Nolex/NIGD/2023.05.10.1200/report-checklist.xlsx
+++ b/GATEWAY/A1#111NOLEXXXXXXX/Nolex/NIGD/2023.05.10.1200/report-checklist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="195">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -698,9 +698,6 @@
     <t>Si è verificato un errore, contattare l'assistenza.</t>
   </si>
   <si>
-    <t>Viene verificato il jwt token e modificato per correggere l'errore.</t>
-  </si>
-  <si>
     <t>2023-05-25T09:59:20Z</t>
   </si>
   <si>
@@ -810,6 +807,23 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.b6c509bc606895ed59d7b22eb303a149a0cb7654837da8fee76aa5b3681e9506.555063760e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Viene verificato il jwt token e modificato per correggere l'errore.Viene gestito in back office.
+Il documento sarà sottoposto nuovamente al medico nella sua worklist di lavoro
+che lo modifica(prendendo atto delle correzioni).
+Verrà messo in coda di invio per il gateway.
+La firma digitale del documento sarà nuovamente applicata dal medico.
+Il documento verrà poi messo in coda di invio per l'fse e verrà inviato successivamente</t>
+  </si>
+  <si>
+    <t>Viene gestito in back office.
+Cancellando il dato errato.
+Il documento sarà sottoposto nuovamente al medico nella sua worklist di lavoro
+che lo modifica(prendendo atto delle correzioni). In questo caso specifico la mancanza del dato forzerà il medico ad inserire il nuovo valore tra un lista di possibili scelte, verrà anche indicato quale valore aveva precedentemente inserito segnalandolo come non compatibile .
+Verrà messo in coda di invio per il gateway.
+La firma digitale del documento sarà nuovamente applicata dal medico.
+Il documento verrà poi messo in coda di invio per l'fse e verrà inviato successivamente</t>
   </si>
 </sst>
 </file>
@@ -3713,10 +3727,10 @@
   <dimension ref="A1:T644"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="J15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomRight" activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -3972,13 +3986,13 @@
         <v>45071</v>
       </c>
       <c r="G9" s="24" t="s">
+        <v>190</v>
+      </c>
+      <c r="H9" s="24" t="s">
         <v>191</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="I9" s="24" t="s">
         <v>192</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>193</v>
       </c>
       <c r="J9" s="25" t="s">
         <v>68</v>
@@ -4110,7 +4124,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="150.75" thickBot="1">
+    <row r="13" spans="1:20" ht="300.75" thickBot="1">
       <c r="A13" s="20">
         <v>29</v>
       </c>
@@ -4155,7 +4169,7 @@
         <v>68</v>
       </c>
       <c r="P13" s="34" t="s">
-        <v>156</v>
+        <v>193</v>
       </c>
       <c r="Q13" s="25"/>
       <c r="R13" s="26"/>
@@ -4164,7 +4178,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="165.75" thickBot="1">
+    <row r="14" spans="1:20" ht="300.75" thickBot="1">
       <c r="A14" s="20">
         <v>37</v>
       </c>
@@ -4184,10 +4198,10 @@
         <v>45071</v>
       </c>
       <c r="G14" s="33" t="s">
+        <v>156</v>
+      </c>
+      <c r="H14" s="33" t="s">
         <v>157</v>
-      </c>
-      <c r="H14" s="33" t="s">
-        <v>158</v>
       </c>
       <c r="I14" s="33" t="s">
         <v>154</v>
@@ -4209,7 +4223,7 @@
         <v>68</v>
       </c>
       <c r="P14" s="34" t="s">
-        <v>156</v>
+        <v>193</v>
       </c>
       <c r="Q14" s="25"/>
       <c r="R14" s="26"/>
@@ -4251,11 +4265,11 @@
         <v>68</v>
       </c>
       <c r="N15" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="O15" s="34"/>
       <c r="P15" s="34" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="26" t="s">
@@ -4266,7 +4280,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="120.75" thickBot="1">
+    <row r="16" spans="1:20" ht="405.75" thickBot="1">
       <c r="A16" s="20">
         <v>63</v>
       </c>
@@ -4286,13 +4300,13 @@
         <v>45071</v>
       </c>
       <c r="G16" s="33" t="s">
+        <v>160</v>
+      </c>
+      <c r="H16" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="H16" s="33" t="s">
+      <c r="I16" s="33" t="s">
         <v>162</v>
-      </c>
-      <c r="I16" s="33" t="s">
-        <v>163</v>
       </c>
       <c r="J16" s="34" t="s">
         <v>68</v>
@@ -4302,16 +4316,16 @@
         <v>68</v>
       </c>
       <c r="M16" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="N16" s="34" t="s">
         <v>164</v>
-      </c>
-      <c r="N16" s="34" t="s">
-        <v>165</v>
       </c>
       <c r="O16" s="34" t="s">
         <v>68</v>
       </c>
       <c r="P16" s="34" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="Q16" s="25"/>
       <c r="R16" s="26"/>
@@ -4340,13 +4354,13 @@
         <v>45071</v>
       </c>
       <c r="G17" s="33" t="s">
+        <v>166</v>
+      </c>
+      <c r="H17" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="H17" s="33" t="s">
+      <c r="I17" s="33" t="s">
         <v>168</v>
-      </c>
-      <c r="I17" s="33" t="s">
-        <v>169</v>
       </c>
       <c r="J17" s="34" t="s">
         <v>68</v>
@@ -4359,13 +4373,13 @@
         <v>68</v>
       </c>
       <c r="N17" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O17" s="34" t="s">
         <v>68</v>
       </c>
       <c r="P17" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q17" s="25"/>
       <c r="R17" s="26"/>
@@ -4374,7 +4388,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="120">
+    <row r="18" spans="1:20" ht="405">
       <c r="A18" s="20">
         <v>65</v>
       </c>
@@ -4394,13 +4408,13 @@
         <v>45071</v>
       </c>
       <c r="G18" s="33" t="s">
+        <v>169</v>
+      </c>
+      <c r="H18" s="33" t="s">
         <v>170</v>
       </c>
-      <c r="H18" s="33" t="s">
+      <c r="I18" s="33" t="s">
         <v>171</v>
-      </c>
-      <c r="I18" s="33" t="s">
-        <v>172</v>
       </c>
       <c r="J18" s="34" t="s">
         <v>68</v>
@@ -4413,13 +4427,13 @@
         <v>68</v>
       </c>
       <c r="N18" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O18" s="34" t="s">
         <v>68</v>
       </c>
       <c r="P18" s="34" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="Q18" s="25"/>
       <c r="R18" s="26"/>
@@ -4448,13 +4462,13 @@
         <v>45071</v>
       </c>
       <c r="G19" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="H19" s="33" t="s">
         <v>173</v>
       </c>
-      <c r="H19" s="33" t="s">
+      <c r="I19" s="33" t="s">
         <v>174</v>
-      </c>
-      <c r="I19" s="33" t="s">
-        <v>175</v>
       </c>
       <c r="J19" s="34" t="s">
         <v>68</v>
@@ -4467,13 +4481,13 @@
         <v>68</v>
       </c>
       <c r="N19" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O19" s="34" t="s">
         <v>68</v>
       </c>
       <c r="P19" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q19" s="25"/>
       <c r="R19" s="26"/>
@@ -4502,13 +4516,13 @@
         <v>45071</v>
       </c>
       <c r="G20" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="H20" s="33" t="s">
         <v>176</v>
       </c>
-      <c r="H20" s="33" t="s">
+      <c r="I20" s="33" t="s">
         <v>177</v>
-      </c>
-      <c r="I20" s="33" t="s">
-        <v>178</v>
       </c>
       <c r="J20" s="34" t="s">
         <v>68</v>
@@ -4521,13 +4535,13 @@
         <v>68</v>
       </c>
       <c r="N20" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O20" s="34" t="s">
         <v>68</v>
       </c>
       <c r="P20" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q20" s="25"/>
       <c r="R20" s="26"/>
@@ -4556,13 +4570,13 @@
         <v>45071</v>
       </c>
       <c r="G21" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="H21" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="H21" s="33" t="s">
+      <c r="I21" s="33" t="s">
         <v>180</v>
-      </c>
-      <c r="I21" s="33" t="s">
-        <v>181</v>
       </c>
       <c r="J21" s="34" t="s">
         <v>68</v>
@@ -4575,13 +4589,13 @@
         <v>68</v>
       </c>
       <c r="N21" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O21" s="34" t="s">
         <v>68</v>
       </c>
       <c r="P21" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q21" s="25"/>
       <c r="R21" s="26"/>
@@ -4610,13 +4624,13 @@
         <v>45071</v>
       </c>
       <c r="G22" s="33" t="s">
+        <v>181</v>
+      </c>
+      <c r="H22" s="33" t="s">
         <v>182</v>
       </c>
-      <c r="H22" s="33" t="s">
+      <c r="I22" s="33" t="s">
         <v>183</v>
-      </c>
-      <c r="I22" s="33" t="s">
-        <v>184</v>
       </c>
       <c r="J22" s="34" t="s">
         <v>68</v>
@@ -4629,13 +4643,13 @@
         <v>68</v>
       </c>
       <c r="N22" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O22" s="34" t="s">
         <v>68</v>
       </c>
       <c r="P22" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q22" s="25"/>
       <c r="R22" s="26"/>
@@ -4664,13 +4678,13 @@
         <v>45071</v>
       </c>
       <c r="G23" s="33" t="s">
+        <v>184</v>
+      </c>
+      <c r="H23" s="33" t="s">
         <v>185</v>
       </c>
-      <c r="H23" s="33" t="s">
+      <c r="I23" s="33" t="s">
         <v>186</v>
-      </c>
-      <c r="I23" s="33" t="s">
-        <v>187</v>
       </c>
       <c r="J23" s="34" t="s">
         <v>68</v>
@@ -4683,13 +4697,13 @@
         <v>68</v>
       </c>
       <c r="N23" s="34" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="O23" s="34" t="s">
         <v>68</v>
       </c>
       <c r="P23" s="34" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="Q23" s="25"/>
       <c r="R23" s="26"/>
@@ -4722,7 +4736,7 @@
         <v>146</v>
       </c>
       <c r="K24" s="34" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L24" s="25"/>
       <c r="M24" s="25"/>
@@ -4760,7 +4774,7 @@
         <v>146</v>
       </c>
       <c r="K25" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L25" s="25"/>
       <c r="M25" s="25"/>
@@ -4798,7 +4812,7 @@
         <v>146</v>
       </c>
       <c r="K26" s="34" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L26" s="25"/>
       <c r="M26" s="25"/>
@@ -4836,7 +4850,7 @@
         <v>146</v>
       </c>
       <c r="K27" s="34" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="L27" s="25"/>
       <c r="M27" s="25"/>

</xml_diff>